<commit_message>
Fix methods to new data
</commit_message>
<xml_diff>
--- a/Data/Results/summary_stats.xlsx
+++ b/Data/Results/summary_stats.xlsx
@@ -447,22 +447,22 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>0.9323292181069966</v>
+        <v>0.8989300411522642</v>
       </c>
       <c r="D2">
-        <v>6.09998353909466</v>
+        <v>6.252181069958859</v>
       </c>
       <c r="E2">
-        <v>0.4980491878266766</v>
+        <v>0.5132522035361657</v>
       </c>
       <c r="F2">
-        <v>13.5019433251865</v>
+        <v>13.02461006533311</v>
       </c>
       <c r="G2">
-        <v>0.03818141692201066</v>
+        <v>0.03831948025187215</v>
       </c>
       <c r="H2">
-        <v>854.0332485121234</v>
+        <v>499.3891749520004</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -473,22 +473,22 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>2.116316425120773</v>
+        <v>2.566919191919193</v>
       </c>
       <c r="D3">
-        <v>7.42661835748792</v>
+        <v>7.480808080808081</v>
       </c>
       <c r="E3">
-        <v>0.9648437284665611</v>
+        <v>1.045814780247639</v>
       </c>
       <c r="F3">
-        <v>58.88417630461714</v>
+        <v>48.00576749879822</v>
       </c>
       <c r="G3">
-        <v>0.03713713284372356</v>
+        <v>0.03748718523446825</v>
       </c>
       <c r="H3">
-        <v>50.29198915522483</v>
+        <v>69.81733537295449</v>
       </c>
     </row>
   </sheetData>
@@ -541,22 +541,22 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>1.657602124183008</v>
+        <v>1.565972222222224</v>
       </c>
       <c r="E2">
-        <v>6.297120098039214</v>
+        <v>6.772140522875823</v>
       </c>
       <c r="F2">
-        <v>0.6393677254552554</v>
+        <v>0.6281495128170839</v>
       </c>
       <c r="G2">
-        <v>9.913023263530036</v>
+        <v>10.01068554655091</v>
       </c>
       <c r="H2">
-        <v>0.04348922817643473</v>
+        <v>0.04290064197226771</v>
       </c>
       <c r="I2">
-        <v>1449.617905560447</v>
+        <v>667.0968282711668</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -570,22 +570,22 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>0.196231343283582</v>
+        <v>0.2219320066334992</v>
       </c>
       <c r="E3">
-        <v>5.899904643449425</v>
+        <v>5.724461028192374</v>
       </c>
       <c r="F3">
-        <v>0.3546214182931939</v>
+        <v>0.3966400090420997</v>
       </c>
       <c r="G3">
-        <v>17.14442935791247</v>
+        <v>16.08351853215685</v>
       </c>
       <c r="H3">
-        <v>0.03279438460408768</v>
+        <v>0.03366994298341094</v>
       </c>
       <c r="I3">
-        <v>249.5592682242724</v>
+        <v>329.1784223295625</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -599,22 +599,22 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>2.203912037037037</v>
+        <v>3.148842592592593</v>
       </c>
       <c r="E4">
-        <v>9.722499999999998</v>
+        <v>9.775000000000002</v>
       </c>
       <c r="F4">
-        <v>0.344114832638416</v>
+        <v>0.3597763375058016</v>
       </c>
       <c r="G4">
-        <v>23.42490357330801</v>
+        <v>22.87505852187092</v>
       </c>
       <c r="H4">
-        <v>0.04564390287892198</v>
+        <v>0.04593606360508246</v>
       </c>
       <c r="I4">
-        <v>82.46945403551952</v>
+        <v>114.7833351028985</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -628,22 +628,22 @@
         <v>11</v>
       </c>
       <c r="D5">
-        <v>2.020757575757576</v>
+        <v>1.868611111111111</v>
       </c>
       <c r="E5">
-        <v>4.922020202020202</v>
+        <v>4.727777777777777</v>
       </c>
       <c r="F5">
-        <v>1.642002523915446</v>
+        <v>1.869060911537844</v>
       </c>
       <c r="G5">
-        <v>97.56701928422709</v>
+        <v>78.16261827111103</v>
       </c>
       <c r="H5">
-        <v>0.02785702007805253</v>
+        <v>0.02734853118973121</v>
       </c>
       <c r="I5">
-        <v>15.18930019490337</v>
+        <v>15.85813569702169</v>
       </c>
     </row>
   </sheetData>
@@ -690,22 +690,22 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>0.8901448611368021</v>
+        <v>0.8571820291471475</v>
       </c>
       <c r="D2">
-        <v>0.4084495831901459</v>
+        <v>0.6504466319630029</v>
       </c>
       <c r="E2">
-        <v>0.1613849369915162</v>
+        <v>0.139794714791673</v>
       </c>
       <c r="F2">
-        <v>4.299797016382755</v>
+        <v>3.778590780298534</v>
       </c>
       <c r="G2">
-        <v>0.006360925606956739</v>
+        <v>0.005683596800217818</v>
       </c>
       <c r="H2">
-        <v>2043.618279421855</v>
+        <v>619.6949162757148</v>
       </c>
     </row>
     <row r="3" spans="1:8">
@@ -716,22 +716,22 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>1.86588235126848</v>
+        <v>1.954582209721116</v>
       </c>
       <c r="D3">
-        <v>2.663471861286584</v>
+        <v>2.754640666345447</v>
       </c>
       <c r="E3">
-        <v>2.223992274760001</v>
+        <v>2.279423883375306</v>
       </c>
       <c r="F3">
-        <v>125.9469353711943</v>
+        <v>83.23337561277928</v>
       </c>
       <c r="G3">
-        <v>0.01318582838321887</v>
+        <v>0.01354971319733675</v>
       </c>
       <c r="H3">
-        <v>51.86930546512156</v>
+        <v>81.68345397934863</v>
       </c>
     </row>
   </sheetData>
@@ -784,22 +784,22 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>0.4013687853378574</v>
+        <v>0.4176650214687206</v>
       </c>
       <c r="E2">
-        <v>0.363272796673333</v>
+        <v>0.2130523963974698</v>
       </c>
       <c r="F2">
-        <v>0.06005260864139923</v>
+        <v>0.04286243121554766</v>
       </c>
       <c r="G2">
-        <v>0.3907507589741741</v>
+        <v>0.3043536084381681</v>
       </c>
       <c r="H2">
-        <v>0.002367757953255067</v>
+        <v>0.001865346479553693</v>
       </c>
       <c r="I2">
-        <v>2747.355795540779</v>
+        <v>789.8194445996253</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -813,22 +813,22 @@
         <v>11</v>
       </c>
       <c r="D3">
-        <v>0.594288008113763</v>
+        <v>0.625300925371889</v>
       </c>
       <c r="E3">
-        <v>0.3522391184125169</v>
+        <v>0.5016420471356491</v>
       </c>
       <c r="F3">
-        <v>0.08808609776334812</v>
+        <v>0.102011886822773</v>
       </c>
       <c r="G3">
-        <v>3.262264279553734</v>
+        <v>3.168031339079627</v>
       </c>
       <c r="H3">
-        <v>0.004239248847993085</v>
+        <v>0.00429935295426457</v>
       </c>
       <c r="I3">
-        <v>283.8767905153113</v>
+        <v>296.6905585105587</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -842,22 +842,22 @@
         <v>10</v>
       </c>
       <c r="D4">
-        <v>2.072983809661067</v>
+        <v>2.132991824232088</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
       <c r="F4">
-        <v>0.1176356292785621</v>
+        <v>0.107722676439064</v>
       </c>
       <c r="G4">
-        <v>3.687257281617022</v>
+        <v>3.696566793870105</v>
       </c>
       <c r="H4">
-        <v>0.001741687068184446</v>
+        <v>0.001633894002878522</v>
       </c>
       <c r="I4">
-        <v>53.55533200126682</v>
+        <v>87.95864472062848</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -871,22 +871,22 @@
         <v>11</v>
       </c>
       <c r="D5">
-        <v>1.706779714006368</v>
+        <v>1.536303958381193</v>
       </c>
       <c r="E5">
-        <v>1.543172398271053</v>
+        <v>1.505449064613414</v>
       </c>
       <c r="F5">
-        <v>3.146351216314069</v>
+        <v>3.27547223484301</v>
       </c>
       <c r="G5">
-        <v>178.1235557402223</v>
+        <v>119.564205707389</v>
       </c>
       <c r="H5">
-        <v>0.01405694942545802</v>
+        <v>0.01468785579066686</v>
       </c>
       <c r="I5">
-        <v>12.88634857497615</v>
+        <v>13.46897201680261</v>
       </c>
     </row>
   </sheetData>

</xml_diff>